<commit_message>
The finished proposal on Oct 20
</commit_message>
<xml_diff>
--- a/data/processed_data/taxa_data.xlsx
+++ b/data/processed_data/taxa_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gufeng/2025_winter/Thesis_Project/ThesisProject/Proposal/data/processed_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A7CFFD-D78A-084E-9D5E-3B48F036CA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C006CBD-C0D1-174A-ACD9-533D0B86A88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-15580" windowWidth="38400" windowHeight="21100" xr2:uid="{A2A3ECF2-71EB-0D46-9A33-44043CB0D53C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A2A3ECF2-71EB-0D46-9A33-44043CB0D53C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="327">
   <si>
     <t>Oligochaeta</t>
   </si>
@@ -1012,7 +1012,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1023,19 +1023,6 @@
     <font>
       <sz val="10"/>
       <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1081,7 +1068,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1092,16 +1079,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1416,10 +1393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF03956-44FD-C74A-BF89-FF787BE89A6A}">
-  <dimension ref="A1:Q384"/>
+  <dimension ref="A1:Q312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" zoomScale="119" workbookViewId="0">
-      <selection activeCell="R247" sqref="R1:R1048576"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="A46" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17958,3822 +17935,6 @@
         <v>3.2034265038149171E-16</v>
       </c>
     </row>
-    <row r="313" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A313" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B313" s="4">
-        <v>2.2699840589301661</v>
-      </c>
-      <c r="C313" s="4">
-        <v>0.563545972426026</v>
-      </c>
-      <c r="D313" s="4">
-        <v>1.6555980433142166</v>
-      </c>
-      <c r="E313" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F313" s="4">
-        <v>0.30911636626288208</v>
-      </c>
-      <c r="G313" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H313" s="4">
-        <v>2.4384391318004006</v>
-      </c>
-      <c r="I313" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J313" s="4">
-        <v>4.5299925551519493</v>
-      </c>
-      <c r="K313" s="4">
-        <v>6.0829184363363407</v>
-      </c>
-      <c r="L313" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M313" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N313" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O313" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P313" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q313" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="314" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A314" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B314" s="4">
-        <v>3.8085037171077323</v>
-      </c>
-      <c r="C314" s="4">
-        <v>3.5120905679098606</v>
-      </c>
-      <c r="D314" s="4">
-        <v>6.2426251710593013</v>
-      </c>
-      <c r="E314" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F314" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G314" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H314" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I314" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J314" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K314" s="4">
-        <v>0.80198174995875249</v>
-      </c>
-      <c r="L314" s="4">
-        <v>0.80198174995875249</v>
-      </c>
-      <c r="M314" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N314" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O314" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P314" s="4">
-        <v>0.45601464350377202</v>
-      </c>
-      <c r="Q314" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="315" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A315" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B315" s="4">
-        <v>0.53852692773087152</v>
-      </c>
-      <c r="C315" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D315" s="4">
-        <v>2.8747658161261094</v>
-      </c>
-      <c r="E315" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F315" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G315" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H315" s="4">
-        <v>0.92977386367496428</v>
-      </c>
-      <c r="I315" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J315" s="4">
-        <v>5.5171616619457922</v>
-      </c>
-      <c r="K315" s="4">
-        <v>5.573081656582537</v>
-      </c>
-      <c r="L315" s="4">
-        <v>0.53852692773087152</v>
-      </c>
-      <c r="M315" s="4">
-        <v>0.53852692773087152</v>
-      </c>
-      <c r="N315" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O315" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P315" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q315" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="316" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A316" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="B316" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="C316" s="4">
-        <v>0.67058292627443994</v>
-      </c>
-      <c r="D316" s="4">
-        <v>1.7514054060243978</v>
-      </c>
-      <c r="E316" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F316" s="4">
-        <v>1.9849829643592762</v>
-      </c>
-      <c r="G316" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H316" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I316" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J316" s="4">
-        <v>4.0854528164864803</v>
-      </c>
-      <c r="K316" s="4">
-        <v>6.294892591337625</v>
-      </c>
-      <c r="L316" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M316" s="4">
-        <v>0.67058292627443994</v>
-      </c>
-      <c r="N316" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O316" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P316" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q316" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="317" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A317" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="B317" s="4">
-        <v>2.5265458144958344</v>
-      </c>
-      <c r="C317" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D317" s="4">
-        <v>3.3955851366126715</v>
-      </c>
-      <c r="E317" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F317" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G317" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H317" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I317" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J317" s="4">
-        <v>3.3955851366126715</v>
-      </c>
-      <c r="K317" s="4">
-        <v>6.2703509527387808</v>
-      </c>
-      <c r="L317" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M317" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N317" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O317" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P317" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q317" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="318" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A318" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B318" s="4">
-        <v>3.8118283986369121</v>
-      </c>
-      <c r="C318" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D318" s="4">
-        <v>3.2773379438632921</v>
-      </c>
-      <c r="E318" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F318" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G318" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H318" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I318" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J318" s="4">
-        <v>3.8118283986369121</v>
-      </c>
-      <c r="K318" s="4">
-        <v>6.0491382704302792</v>
-      </c>
-      <c r="L318" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M318" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N318" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O318" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P318" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q318" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="319" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A319" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B319" s="4">
-        <v>0.70353629593624023</v>
-      </c>
-      <c r="C319" s="4">
-        <v>0.18860956470723933</v>
-      </c>
-      <c r="D319" s="4">
-        <v>0.64030553456493144</v>
-      </c>
-      <c r="E319" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F319" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G319" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H319" s="4">
-        <v>9.7384804660700902E-2</v>
-      </c>
-      <c r="I319" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J319" s="4">
-        <v>5.4622680581916896</v>
-      </c>
-      <c r="K319" s="4">
-        <v>5.584878542561218</v>
-      </c>
-      <c r="L319" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M319" s="4">
-        <v>3.1636426491906642</v>
-      </c>
-      <c r="N319" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O319" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P319" s="4">
-        <v>0.64030553456493144</v>
-      </c>
-      <c r="Q319" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="320" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A320" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="B320" s="4">
-        <v>3.025535092107138</v>
-      </c>
-      <c r="C320" s="4">
-        <v>1.4780472968046441</v>
-      </c>
-      <c r="D320" s="4">
-        <v>2.1926450779423958</v>
-      </c>
-      <c r="E320" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F320" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G320" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H320" s="4">
-        <v>1.4780472968046441</v>
-      </c>
-      <c r="I320" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J320" s="4">
-        <v>3.5501970825604796</v>
-      </c>
-      <c r="K320" s="4">
-        <v>5.9886846867721655</v>
-      </c>
-      <c r="L320" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M320" s="4">
-        <v>3.025535092107138</v>
-      </c>
-      <c r="N320" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O320" s="4">
-        <v>2.6683785089087935</v>
-      </c>
-      <c r="P320" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q320" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="321" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A321" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B321" s="4">
-        <v>4.1429579538420427</v>
-      </c>
-      <c r="C321" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D321" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="E321" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F321" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G321" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H321" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I321" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J321" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K321" s="4">
-        <v>6.3980310739731543</v>
-      </c>
-      <c r="L321" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M321" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N321" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O321" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P321" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q321" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="322" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A322" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B322" s="4">
-        <v>1.4712009112558775</v>
-      </c>
-      <c r="C322" s="4">
-        <v>0.85790751008790844</v>
-      </c>
-      <c r="D322" s="4">
-        <v>1.2649865120975314</v>
-      </c>
-      <c r="E322" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F322" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G322" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H322" s="4">
-        <v>1.68511366861321</v>
-      </c>
-      <c r="I322" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J322" s="4">
-        <v>4.0452333647353615</v>
-      </c>
-      <c r="K322" s="4">
-        <v>6.3090043977422727</v>
-      </c>
-      <c r="L322" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M322" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N322" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O322" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P322" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q322" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="323" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A323" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="B323" s="4">
-        <v>1.0413839207651192</v>
-      </c>
-      <c r="C323" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D323" s="4">
-        <v>2.0616390657923862</v>
-      </c>
-      <c r="E323" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F323" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G323" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H323" s="4">
-        <v>3.4663543528460359</v>
-      </c>
-      <c r="I323" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J323" s="4">
-        <v>3.9341120643435432</v>
-      </c>
-      <c r="K323" s="4">
-        <v>6.1784870149457367</v>
-      </c>
-      <c r="L323" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M323" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N323" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O323" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P323" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q323" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="324" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A324" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="B324" s="4">
-        <v>5.368130103004817</v>
-      </c>
-      <c r="C324" s="4">
-        <v>0.51705843621935277</v>
-      </c>
-      <c r="D324" s="4">
-        <v>5.6353741263673349</v>
-      </c>
-      <c r="E324" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F324" s="4">
-        <v>2.7695528893452201</v>
-      </c>
-      <c r="G324" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H324" s="4">
-        <v>1.1973014403736177</v>
-      </c>
-      <c r="I324" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J324" s="4">
-        <v>1.5556469338966004</v>
-      </c>
-      <c r="K324" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L324" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M324" s="4">
-        <v>0.89690650703589658</v>
-      </c>
-      <c r="N324" s="4">
-        <v>0.71944783290817693</v>
-      </c>
-      <c r="O324" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P324" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q324" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="325" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A325" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="B325" s="4">
-        <v>1.9629379057784551</v>
-      </c>
-      <c r="C325" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D325" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="E325" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F325" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G325" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H325" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I325" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J325" s="4">
-        <v>5.8819341082955416</v>
-      </c>
-      <c r="K325" s="4">
-        <v>5.2735591333637979</v>
-      </c>
-      <c r="L325" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M325" s="4">
-        <v>1.2923549795040155</v>
-      </c>
-      <c r="N325" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O325" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P325" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q325" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="326" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A326" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="B326" s="4">
-        <v>3.6898316185751114</v>
-      </c>
-      <c r="C326" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D326" s="4">
-        <v>2.5265458144958344</v>
-      </c>
-      <c r="E326" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F326" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G326" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H326" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I326" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J326" s="4">
-        <v>3.9341120643435432</v>
-      </c>
-      <c r="K326" s="4">
-        <v>6.1302641084760703</v>
-      </c>
-      <c r="L326" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M326" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N326" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O326" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P326" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q326" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="327" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A327" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B327" s="4">
-        <v>3.9341120643435432</v>
-      </c>
-      <c r="C327" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D327" s="4">
-        <v>6.4381977841980778</v>
-      </c>
-      <c r="E327" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F327" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G327" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H327" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I327" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J327" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K327" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L327" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M327" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N327" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O327" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P327" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q327" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="328" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A328" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B328" s="4">
-        <v>0.13142399528133136</v>
-      </c>
-      <c r="C328" s="4">
-        <v>0.25186895983161989</v>
-      </c>
-      <c r="D328" s="4">
-        <v>6.7208008326684263E-2</v>
-      </c>
-      <c r="E328" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F328" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G328" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H328" s="4">
-        <v>6.7208008326684263E-2</v>
-      </c>
-      <c r="I328" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J328" s="4">
-        <v>5.1312865966882075</v>
-      </c>
-      <c r="K328" s="4">
-        <v>5.8493077735987038</v>
-      </c>
-      <c r="L328" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M328" s="4">
-        <v>2.8189059414801068</v>
-      </c>
-      <c r="N328" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O328" s="4">
-        <v>1.949060616091415</v>
-      </c>
-      <c r="P328" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q328" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="329" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A329" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B329" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="C329" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D329" s="4">
-        <v>0.46501471441365166</v>
-      </c>
-      <c r="E329" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F329" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G329" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H329" s="4">
-        <v>1.1697072460133315</v>
-      </c>
-      <c r="I329" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J329" s="4">
-        <v>5.4878061898718036</v>
-      </c>
-      <c r="K329" s="4">
-        <v>5.7396160355454606</v>
-      </c>
-      <c r="L329" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M329" s="4">
-        <v>1.615725305729703</v>
-      </c>
-      <c r="N329" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O329" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P329" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q329" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="330" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A330" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="B330" s="4">
-        <v>0.86177574934056855</v>
-      </c>
-      <c r="C330" s="4">
-        <v>0.44703192300794964</v>
-      </c>
-      <c r="D330" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="E330" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F330" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G330" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H330" s="4">
-        <v>0.8537433526606869</v>
-      </c>
-      <c r="I330" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J330" s="4">
-        <v>3.5151134818251504</v>
-      </c>
-      <c r="K330" s="4">
-        <v>6.417717158593554</v>
-      </c>
-      <c r="L330" s="4">
-        <v>0.86177574934056855</v>
-      </c>
-      <c r="M330" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N330" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O330" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P330" s="4">
-        <v>1.7093809989535156</v>
-      </c>
-      <c r="Q330" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="331" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A331" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B331" s="4">
-        <v>4.7004397181410917</v>
-      </c>
-      <c r="C331" s="4">
-        <v>5.266786540694901</v>
-      </c>
-      <c r="D331" s="4">
-        <v>3.7548875021634687</v>
-      </c>
-      <c r="E331" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F331" s="4">
-        <v>3.7548875021634687</v>
-      </c>
-      <c r="G331" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H331" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I331" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J331" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K331" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L331" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M331" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N331" s="4">
-        <v>3.7548875021634687</v>
-      </c>
-      <c r="O331" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P331" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q331" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="332" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A332" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B332" s="4">
-        <v>5.6724253419714952</v>
-      </c>
-      <c r="C332" s="4">
-        <v>2.9668331360648006</v>
-      </c>
-      <c r="D332" s="4">
-        <v>1.7104933828050153</v>
-      </c>
-      <c r="E332" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F332" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G332" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H332" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I332" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J332" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K332" s="4">
-        <v>5.3891913217920413</v>
-      </c>
-      <c r="L332" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M332" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N332" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O332" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P332" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q332" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="333" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A333" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B333" s="4">
-        <v>5.966671823933936</v>
-      </c>
-      <c r="C333" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D333" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="E333" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F333" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G333" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H333" s="4">
-        <v>2.2768402053588246</v>
-      </c>
-      <c r="I333" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J333" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K333" s="4">
-        <v>5.154428665119144</v>
-      </c>
-      <c r="L333" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M333" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N333" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O333" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P333" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q333" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="334" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A334" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B334" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="C334" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D334" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="E334" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F334" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G334" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H334" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I334" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J334" s="4">
-        <v>3.3016987698845663</v>
-      </c>
-      <c r="K334" s="4">
-        <v>6.5257438009012416</v>
-      </c>
-      <c r="L334" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M334" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N334" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O334" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P334" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q334" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="335" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A335" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B335" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="C335" s="4">
-        <v>4.7602307048182572E-2</v>
-      </c>
-      <c r="D335" s="4">
-        <v>9.3683996548344778E-2</v>
-      </c>
-      <c r="E335" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F335" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G335" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H335" s="4">
-        <v>9.3683996548344778E-2</v>
-      </c>
-      <c r="I335" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J335" s="4">
-        <v>0.9047272710591775</v>
-      </c>
-      <c r="K335" s="4">
-        <v>6.6432801582885794</v>
-      </c>
-      <c r="L335" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M335" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N335" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O335" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P335" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q335" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="336" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A336" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B336" s="4">
-        <v>1.0297473433940518</v>
-      </c>
-      <c r="C336" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D336" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="E336" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F336" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G336" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H336" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I336" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J336" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K336" s="4">
-        <v>6.6432549415722786</v>
-      </c>
-      <c r="L336" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M336" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N336" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O336" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P336" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q336" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="337" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A337" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B337" s="4">
-        <v>3.9619319591664808</v>
-      </c>
-      <c r="C337" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D337" s="4">
-        <v>3.9619319591664808</v>
-      </c>
-      <c r="E337" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F337" s="4">
-        <v>3.2223924213364481</v>
-      </c>
-      <c r="G337" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H337" s="4">
-        <v>2.3692338096657193</v>
-      </c>
-      <c r="I337" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J337" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K337" s="4">
-        <v>5.8907709302452416</v>
-      </c>
-      <c r="L337" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M337" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N337" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O337" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P337" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q337" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="338" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A338" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B338" s="4">
-        <v>1.9274179978651003</v>
-      </c>
-      <c r="C338" s="4">
-        <v>0.95201997109817849</v>
-      </c>
-      <c r="D338" s="4">
-        <v>2.9149578768766329</v>
-      </c>
-      <c r="E338" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F338" s="4">
-        <v>1.9274179978651003</v>
-      </c>
-      <c r="G338" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H338" s="4">
-        <v>0.95201997109817849</v>
-      </c>
-      <c r="I338" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J338" s="4">
-        <v>2.7240994184082523</v>
-      </c>
-      <c r="K338" s="4">
-        <v>6.3464930216018773</v>
-      </c>
-      <c r="L338" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M338" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N338" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O338" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P338" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q338" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="339" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A339" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B339" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="C339" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D339" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="E339" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F339" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G339" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H339" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I339" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J339" s="4">
-        <v>4</v>
-      </c>
-      <c r="K339" s="4">
-        <v>6.4262647547020979</v>
-      </c>
-      <c r="L339" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M339" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N339" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O339" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P339" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q339" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="340" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A340" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B340" s="4">
-        <v>4.3923174227787607</v>
-      </c>
-      <c r="C340" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D340" s="4">
-        <v>5.9307373375628867</v>
-      </c>
-      <c r="E340" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F340" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G340" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H340" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I340" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J340" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K340" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L340" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M340" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N340" s="4">
-        <v>4.3923174227787607</v>
-      </c>
-      <c r="O340" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P340" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q340" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="341" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A341" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B341" s="4">
-        <v>5.427236921208487</v>
-      </c>
-      <c r="C341" s="4">
-        <v>3.9535216809423219</v>
-      </c>
-      <c r="D341" s="4">
-        <v>3.043760385528413</v>
-      </c>
-      <c r="E341" s="4">
-        <v>4.8347229391233846</v>
-      </c>
-      <c r="F341" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G341" s="4">
-        <v>1.2923549795040155</v>
-      </c>
-      <c r="H341" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I341" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J341" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K341" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L341" s="4">
-        <v>3.043760385528413</v>
-      </c>
-      <c r="M341" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N341" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O341" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P341" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q341" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="342" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A342" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B342" s="4">
-        <v>0.65207669657969336</v>
-      </c>
-      <c r="C342" s="4">
-        <v>0.1926450779423961</v>
-      </c>
-      <c r="D342" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="E342" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F342" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G342" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H342" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I342" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J342" s="4">
-        <v>5.1584293626044833</v>
-      </c>
-      <c r="K342" s="4">
-        <v>6.0032167126835425</v>
-      </c>
-      <c r="L342" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M342" s="4">
-        <v>1.2801079191927354</v>
-      </c>
-      <c r="N342" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O342" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P342" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q342" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="343" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A343" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B343" s="4">
-        <v>5.036423408249874</v>
-      </c>
-      <c r="C343" s="4">
-        <v>5.6289149562032419</v>
-      </c>
-      <c r="D343" s="4">
-        <v>4.013597603400723</v>
-      </c>
-      <c r="E343" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F343" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G343" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H343" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I343" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J343" s="4">
-        <v>2.0108883161427364</v>
-      </c>
-      <c r="K343" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L343" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M343" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N343" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O343" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P343" s="4">
-        <v>1.3306453119884716</v>
-      </c>
-      <c r="Q343" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="344" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A344" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B344" s="4">
-        <v>4.4432563430885725</v>
-      </c>
-      <c r="C344" s="4">
-        <v>5.203555779323592</v>
-      </c>
-      <c r="D344" s="4">
-        <v>3.6230187269832319</v>
-      </c>
-      <c r="E344" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F344" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G344" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H344" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I344" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J344" s="4">
-        <v>4.7768985330696419</v>
-      </c>
-      <c r="K344" s="4">
-        <v>2.2550731201311112</v>
-      </c>
-      <c r="L344" s="4">
-        <v>1.5294673881294527</v>
-      </c>
-      <c r="M344" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N344" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O344" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P344" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q344" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="345" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A345" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="B345" s="4">
-        <v>6.2479275134435852</v>
-      </c>
-      <c r="C345" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D345" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="E345" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F345" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G345" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H345" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I345" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J345" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K345" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L345" s="4">
-        <v>4.7004397181410917</v>
-      </c>
-      <c r="M345" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N345" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O345" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P345" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q345" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="346" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A346" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="B346" s="4">
-        <v>6.6582114827517946</v>
-      </c>
-      <c r="C346" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D346" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="E346" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F346" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G346" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H346" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I346" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J346" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K346" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L346" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M346" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N346" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O346" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P346" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q346" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="347" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A347" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B347" s="4">
-        <v>6.6476700428896072</v>
-      </c>
-      <c r="C347" s="4">
-        <v>0.79518020811150203</v>
-      </c>
-      <c r="D347" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="E347" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F347" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G347" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H347" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I347" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J347" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K347" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L347" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M347" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N347" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O347" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P347" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q347" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="348" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A348" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="B348" s="4">
-        <v>6.6582114827517946</v>
-      </c>
-      <c r="C348" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D348" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="E348" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F348" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G348" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H348" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I348" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J348" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K348" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L348" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M348" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N348" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O348" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P348" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q348" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="349" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A349" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="B349" s="4">
-        <v>6.6582114827517946</v>
-      </c>
-      <c r="C349" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D349" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="E349" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F349" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G349" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H349" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I349" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J349" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K349" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L349" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M349" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N349" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O349" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P349" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q349" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="350" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A350" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B350" s="4">
-        <v>0.68684211474036982</v>
-      </c>
-      <c r="C350" s="4">
-        <v>1.1502426355806128</v>
-      </c>
-      <c r="D350" s="4">
-        <v>0.68684211474036982</v>
-      </c>
-      <c r="E350" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F350" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G350" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H350" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I350" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J350" s="4">
-        <v>3.5820272096966095</v>
-      </c>
-      <c r="K350" s="4">
-        <v>6.4526179330465743</v>
-      </c>
-      <c r="L350" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M350" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N350" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O350" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P350" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q350" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="351" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A351" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B351" s="4">
-        <v>6.5415901494393482</v>
-      </c>
-      <c r="C351" s="4">
-        <v>2.5611943347882069</v>
-      </c>
-      <c r="D351" s="4">
-        <v>1.5659793973535834</v>
-      </c>
-      <c r="E351" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F351" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G351" s="4">
-        <v>0.98578614078029925</v>
-      </c>
-      <c r="H351" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I351" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J351" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K351" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L351" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M351" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N351" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O351" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P351" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q351" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="352" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A352" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B352" s="4">
-        <v>3.1315853944826477</v>
-      </c>
-      <c r="C352" s="4">
-        <v>4.2009518970629367</v>
-      </c>
-      <c r="D352" s="4">
-        <v>4.7090302820544769</v>
-      </c>
-      <c r="E352" s="4">
-        <v>1.5177060623147212</v>
-      </c>
-      <c r="F352" s="4">
-        <v>0.39018231059256858</v>
-      </c>
-      <c r="G352" s="4">
-        <v>1.8009400824941761</v>
-      </c>
-      <c r="H352" s="4">
-        <v>0.69698911845526779</v>
-      </c>
-      <c r="I352" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J352" s="4">
-        <v>2.5774757426591339</v>
-      </c>
-      <c r="K352" s="4">
-        <v>5.3266248815887609</v>
-      </c>
-      <c r="L352" s="4">
-        <v>0.39018231059256858</v>
-      </c>
-      <c r="M352" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N352" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O352" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P352" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q352" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="353" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A353" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B353" s="4">
-        <v>6.4457633258026634</v>
-      </c>
-      <c r="C353" s="4">
-        <v>3.7453822955509679</v>
-      </c>
-      <c r="D353" s="4">
-        <v>1.0453239905094907</v>
-      </c>
-      <c r="E353" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F353" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G353" s="4">
-        <v>0.43787747563695545</v>
-      </c>
-      <c r="H353" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I353" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J353" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K353" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L353" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M353" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N353" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O353" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P353" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q353" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="354" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A354" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B354" s="4">
-        <v>5.6893665305441177</v>
-      </c>
-      <c r="C354" s="4">
-        <v>5.5846003330172609</v>
-      </c>
-      <c r="D354" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="E354" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F354" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G354" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H354" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I354" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J354" s="4">
-        <v>1.7696188114849576</v>
-      </c>
-      <c r="K354" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L354" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M354" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N354" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O354" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P354" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q354" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="355" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A355" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B355" s="4">
-        <v>6.5810023142079004</v>
-      </c>
-      <c r="C355" s="4">
-        <v>2.6468902498643581</v>
-      </c>
-      <c r="D355" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="E355" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F355" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G355" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H355" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I355" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J355" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K355" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L355" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M355" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N355" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O355" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P355" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q355" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="356" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A356" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B356" s="4">
-        <v>6.2368485537537088</v>
-      </c>
-      <c r="C356" s="4">
-        <v>4.5293851528262756</v>
-      </c>
-      <c r="D356" s="4">
-        <v>1.7336065820762918</v>
-      </c>
-      <c r="E356" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F356" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G356" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H356" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I356" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J356" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K356" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L356" s="4">
-        <v>1.1128940564059338</v>
-      </c>
-      <c r="M356" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N356" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O356" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P356" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q356" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="357" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A357" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B357" s="4">
-        <v>6.5077946401986964</v>
-      </c>
-      <c r="C357" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D357" s="4">
-        <v>2.5849625007211565</v>
-      </c>
-      <c r="E357" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F357" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G357" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H357" s="4">
-        <v>2.5849625007211565</v>
-      </c>
-      <c r="I357" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J357" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K357" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L357" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M357" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N357" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O357" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P357" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q357" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="358" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A358" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="B358" s="4">
-        <v>4.287798241703582</v>
-      </c>
-      <c r="C358" s="4">
-        <v>0.2113454590115004</v>
-      </c>
-      <c r="D358" s="4">
-        <v>1.550047801978546</v>
-      </c>
-      <c r="E358" s="4">
-        <v>3.0033247236745504E-2</v>
-      </c>
-      <c r="F358" s="4">
-        <v>0.2113454590115004</v>
-      </c>
-      <c r="G358" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H358" s="4">
-        <v>0.37239404702112239</v>
-      </c>
-      <c r="I358" s="4">
-        <v>0.41853592327376271</v>
-      </c>
-      <c r="J358" s="4">
-        <v>5.7943215382903661</v>
-      </c>
-      <c r="K358" s="4">
-        <v>1.2325305341640147</v>
-      </c>
-      <c r="L358" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M358" s="4">
-        <v>4.3047887958438578</v>
-      </c>
-      <c r="N358" s="4">
-        <v>0.12585540096522971</v>
-      </c>
-      <c r="O358" s="4">
-        <v>1.299817901035019</v>
-      </c>
-      <c r="P358" s="4">
-        <v>0.53830631247269722</v>
-      </c>
-      <c r="Q358" s="4">
-        <v>1.563800465403655</v>
-      </c>
-    </row>
-    <row r="359" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A359" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B359" s="4">
-        <v>6.5667915595511097</v>
-      </c>
-      <c r="C359" s="4">
-        <v>2.2856889514560352</v>
-      </c>
-      <c r="D359" s="4">
-        <v>1.3507165183119876</v>
-      </c>
-      <c r="E359" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F359" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G359" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H359" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I359" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J359" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K359" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L359" s="4">
-        <v>0.82797653267368998</v>
-      </c>
-      <c r="M359" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N359" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O359" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P359" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q359" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="360" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A360" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="B360" s="4">
-        <v>6.4555557980043803</v>
-      </c>
-      <c r="C360" s="4">
-        <v>0.60216557225367406</v>
-      </c>
-      <c r="D360" s="4">
-        <v>0.11341838679182119</v>
-      </c>
-      <c r="E360" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F360" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G360" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H360" s="4">
-        <v>0.60216557225367406</v>
-      </c>
-      <c r="I360" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J360" s="4">
-        <v>1.782417711857881</v>
-      </c>
-      <c r="K360" s="4">
-        <v>0.33227453417906111</v>
-      </c>
-      <c r="L360" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M360" s="4">
-        <v>2.0527132234898589</v>
-      </c>
-      <c r="N360" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O360" s="4">
-        <v>0.60216557225367406</v>
-      </c>
-      <c r="P360" s="4">
-        <v>1.1372174450179071</v>
-      </c>
-      <c r="Q360" s="4">
-        <v>2.4732387803063038</v>
-      </c>
-    </row>
-    <row r="361" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A361" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="B361" s="4">
-        <v>2.7117527503773009</v>
-      </c>
-      <c r="C361" s="4">
-        <v>0.4244010755349773</v>
-      </c>
-      <c r="D361" s="4">
-        <v>2.5591122065613825</v>
-      </c>
-      <c r="E361" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F361" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G361" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H361" s="4">
-        <v>1.5200095559618199</v>
-      </c>
-      <c r="I361" s="4">
-        <v>0.4244010755349773</v>
-      </c>
-      <c r="J361" s="4">
-        <v>2.5133105944678418</v>
-      </c>
-      <c r="K361" s="4">
-        <v>2.8550331490088068</v>
-      </c>
-      <c r="L361" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M361" s="4">
-        <v>6.0055462727301663</v>
-      </c>
-      <c r="N361" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O361" s="4">
-        <v>2.5972456553649108</v>
-      </c>
-      <c r="P361" s="4">
-        <v>1.6706753432558392</v>
-      </c>
-      <c r="Q361" s="4">
-        <v>2.7175348712223566</v>
-      </c>
-    </row>
-    <row r="362" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A362" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B362" s="4">
-        <v>5.525324026912509</v>
-      </c>
-      <c r="C362" s="4">
-        <v>0.36471212153635268</v>
-      </c>
-      <c r="D362" s="4">
-        <v>2.3677119123455337</v>
-      </c>
-      <c r="E362" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F362" s="4">
-        <v>0.36471212153635268</v>
-      </c>
-      <c r="G362" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H362" s="4">
-        <v>2.9408938218850724</v>
-      </c>
-      <c r="I362" s="4">
-        <v>1.2702153398251084</v>
-      </c>
-      <c r="J362" s="4">
-        <v>4.730438893841046</v>
-      </c>
-      <c r="K362" s="4">
-        <v>2.3894738378555598</v>
-      </c>
-      <c r="L362" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M362" s="4">
-        <v>2.2727713215419256</v>
-      </c>
-      <c r="N362" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O362" s="4">
-        <v>1.2271269832436231</v>
-      </c>
-      <c r="P362" s="4">
-        <v>1.0844831241681252</v>
-      </c>
-      <c r="Q362" s="4">
-        <v>2.8148339416483821</v>
-      </c>
-    </row>
-    <row r="363" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A363" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B363" s="4">
-        <v>5.7348490596842225</v>
-      </c>
-      <c r="C363" s="4">
-        <v>2.2902673070250041</v>
-      </c>
-      <c r="D363" s="4">
-        <v>2.9746476981431424</v>
-      </c>
-      <c r="E363" s="4">
-        <v>0.54415862979710794</v>
-      </c>
-      <c r="F363" s="4">
-        <v>0.34228337694646527</v>
-      </c>
-      <c r="G363" s="4">
-        <v>0.20752638852383118</v>
-      </c>
-      <c r="H363" s="4">
-        <v>0.61873014787014335</v>
-      </c>
-      <c r="I363" s="4">
-        <v>0.33549612769068854</v>
-      </c>
-      <c r="J363" s="4">
-        <v>3.5923404981565423</v>
-      </c>
-      <c r="K363" s="4">
-        <v>4.2879928219582153</v>
-      </c>
-      <c r="L363" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M363" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N363" s="4">
-        <v>0.20752638852383118</v>
-      </c>
-      <c r="O363" s="4">
-        <v>1.0462087093486641</v>
-      </c>
-      <c r="P363" s="4">
-        <v>0.65188938832003995</v>
-      </c>
-      <c r="Q363" s="4">
-        <v>2.3007589178096812</v>
-      </c>
-    </row>
-    <row r="364" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A364" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="B364" s="4">
-        <v>3.6485459845174129</v>
-      </c>
-      <c r="C364" s="4">
-        <v>0.56373505594642681</v>
-      </c>
-      <c r="D364" s="4">
-        <v>1.8204050539787764</v>
-      </c>
-      <c r="E364" s="4">
-        <v>7.0235092190285092E-2</v>
-      </c>
-      <c r="F364" s="4">
-        <v>0.10411068095961228</v>
-      </c>
-      <c r="G364" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H364" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I364" s="4">
-        <v>0.48450116553101463</v>
-      </c>
-      <c r="J364" s="4">
-        <v>1.7310878527627203</v>
-      </c>
-      <c r="K364" s="4">
-        <v>6.3656670402005044</v>
-      </c>
-      <c r="L364" s="4">
-        <v>3.5544913016885865E-2</v>
-      </c>
-      <c r="M364" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N364" s="4">
-        <v>0.4541767687672057</v>
-      </c>
-      <c r="O364" s="4">
-        <v>0.53918073814255851</v>
-      </c>
-      <c r="P364" s="4">
-        <v>0.24741603700972165</v>
-      </c>
-      <c r="Q364" s="4">
-        <v>0.14807523300635292</v>
-      </c>
-    </row>
-    <row r="365" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A365" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B365" s="4">
-        <v>1.5670449940914724</v>
-      </c>
-      <c r="C365" s="4">
-        <v>0.41653319095267272</v>
-      </c>
-      <c r="D365" s="4">
-        <v>1.2236565887380222</v>
-      </c>
-      <c r="E365" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F365" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G365" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H365" s="4">
-        <v>0.21026204016452632</v>
-      </c>
-      <c r="I365" s="4">
-        <v>0.12057187084235274</v>
-      </c>
-      <c r="J365" s="4">
-        <v>1.0523335759776689</v>
-      </c>
-      <c r="K365" s="4">
-        <v>6.5341459321289959</v>
-      </c>
-      <c r="L365" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M365" s="4">
-        <v>2.9869498814956513E-2</v>
-      </c>
-      <c r="N365" s="4">
-        <v>2.9869498814956513E-2</v>
-      </c>
-      <c r="O365" s="4">
-        <v>1.490344382923031</v>
-      </c>
-      <c r="P365" s="4">
-        <v>1.3214954378018318</v>
-      </c>
-      <c r="Q365" s="4">
-        <v>2.9869498814956513E-2</v>
-      </c>
-    </row>
-    <row r="366" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A366" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="B366" s="4">
-        <v>1.3595858074949612</v>
-      </c>
-      <c r="C366" s="4">
-        <v>7.2822538035827486E-2</v>
-      </c>
-      <c r="D366" s="4">
-        <v>0.12726292462738834</v>
-      </c>
-      <c r="E366" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F366" s="4">
-        <v>1.393717104658746E-2</v>
-      </c>
-      <c r="G366" s="4">
-        <v>0.18178273305015352</v>
-      </c>
-      <c r="H366" s="4">
-        <v>4.3680268495449481E-2</v>
-      </c>
-      <c r="I366" s="4">
-        <v>4.3680268495449481E-2</v>
-      </c>
-      <c r="J366" s="4">
-        <v>1.1919432129966827</v>
-      </c>
-      <c r="K366" s="4">
-        <v>6.5870628929722104</v>
-      </c>
-      <c r="L366" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M366" s="4">
-        <v>0.40267807158027352</v>
-      </c>
-      <c r="N366" s="4">
-        <v>1.393717104658746E-2</v>
-      </c>
-      <c r="O366" s="4">
-        <v>0.18178273305015352</v>
-      </c>
-      <c r="P366" s="4">
-        <v>0.68990680794708548</v>
-      </c>
-      <c r="Q366" s="4">
-        <v>0.66067453125684339</v>
-      </c>
-    </row>
-    <row r="367" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A367" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="B367" s="4">
-        <v>5.9321160495358676</v>
-      </c>
-      <c r="C367" s="4">
-        <v>0.98644716823597789</v>
-      </c>
-      <c r="D367" s="4">
-        <v>1.6046827497858562</v>
-      </c>
-      <c r="E367" s="4">
-        <v>3.9521144809592422E-2</v>
-      </c>
-      <c r="F367" s="4">
-        <v>3.9521144809592422E-2</v>
-      </c>
-      <c r="G367" s="4">
-        <v>0.27297243913987401</v>
-      </c>
-      <c r="H367" s="4">
-        <v>3.9521144809592422E-2</v>
-      </c>
-      <c r="I367" s="4">
-        <v>0.49296268607356547</v>
-      </c>
-      <c r="J367" s="4">
-        <v>1.7801985046648652</v>
-      </c>
-      <c r="K367" s="4">
-        <v>3.5093114153145688</v>
-      </c>
-      <c r="L367" s="4">
-        <v>0.27297243913987401</v>
-      </c>
-      <c r="M367" s="4">
-        <v>4.0891745122027379</v>
-      </c>
-      <c r="N367" s="4">
-        <v>0.19344620431609044</v>
-      </c>
-      <c r="O367" s="4">
-        <v>2.6372057163149663</v>
-      </c>
-      <c r="P367" s="4">
-        <v>0.4642075146304509</v>
-      </c>
-      <c r="Q367" s="4">
-        <v>1.2783784835494212</v>
-      </c>
-    </row>
-    <row r="368" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A368" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B368" s="4">
-        <v>1.6878958967021915</v>
-      </c>
-      <c r="C368" s="4">
-        <v>0.58238569314074407</v>
-      </c>
-      <c r="D368" s="4">
-        <v>5.1814601347553349E-2</v>
-      </c>
-      <c r="E368" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F368" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G368" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H368" s="4">
-        <v>3.9547755563313004E-2</v>
-      </c>
-      <c r="I368" s="4">
-        <v>8.9985489184973705E-2</v>
-      </c>
-      <c r="J368" s="4">
-        <v>1.9413291891216113</v>
-      </c>
-      <c r="K368" s="4">
-        <v>6.3613182594506847</v>
-      </c>
-      <c r="L368" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M368" s="4">
-        <v>3.1710312872328776</v>
-      </c>
-      <c r="N368" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O368" s="4">
-        <v>1.916389157156134</v>
-      </c>
-      <c r="P368" s="4">
-        <v>1.5236628776337666</v>
-      </c>
-      <c r="Q368" s="4">
-        <v>0.52634663479255506</v>
-      </c>
-    </row>
-    <row r="369" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A369" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B369" s="4">
-        <v>6.4119013132209437</v>
-      </c>
-      <c r="C369" s="4">
-        <v>2.9861687984311471</v>
-      </c>
-      <c r="D369" s="4">
-        <v>2.565364168508903</v>
-      </c>
-      <c r="E369" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F369" s="4">
-        <v>0.26359046482733772</v>
-      </c>
-      <c r="G369" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H369" s="4">
-        <v>0.66536331427323481</v>
-      </c>
-      <c r="I369" s="4">
-        <v>0.24493868543907196</v>
-      </c>
-      <c r="J369" s="4">
-        <v>1.1291876710226594</v>
-      </c>
-      <c r="K369" s="4">
-        <v>0.12766127866631943</v>
-      </c>
-      <c r="L369" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M369" s="4">
-        <v>0.12766127866631943</v>
-      </c>
-      <c r="N369" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O369" s="4">
-        <v>0.48637993998241663</v>
-      </c>
-      <c r="P369" s="4">
-        <v>0.56367185741645121</v>
-      </c>
-      <c r="Q369" s="4">
-        <v>0.83707956461312227</v>
-      </c>
-    </row>
-    <row r="370" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A370" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B370" s="4">
-        <v>3.1726279437615519</v>
-      </c>
-      <c r="C370" s="4">
-        <v>2.6971582007925123</v>
-      </c>
-      <c r="D370" s="4">
-        <v>2.6971582007925123</v>
-      </c>
-      <c r="E370" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F370" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G370" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H370" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I370" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J370" s="4">
-        <v>5.5543297934903926</v>
-      </c>
-      <c r="K370" s="4">
-        <v>4.3210147076831342</v>
-      </c>
-      <c r="L370" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M370" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N370" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O370" s="4">
-        <v>3.8581908874740383</v>
-      </c>
-      <c r="P370" s="4">
-        <v>1.8203405636520849</v>
-      </c>
-      <c r="Q370" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="371" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A371" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B371" s="4">
-        <v>5.3268398064316314</v>
-      </c>
-      <c r="C371" s="4">
-        <v>4.4107160421215479</v>
-      </c>
-      <c r="D371" s="4">
-        <v>3.3869414306287209</v>
-      </c>
-      <c r="E371" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F371" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G371" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H371" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I371" s="4">
-        <v>0.22035038979822938</v>
-      </c>
-      <c r="J371" s="4">
-        <v>4.5910995317617482</v>
-      </c>
-      <c r="K371" s="4">
-        <v>0.22035038979822938</v>
-      </c>
-      <c r="L371" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M371" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N371" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O371" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P371" s="4">
-        <v>0.73124060633257637</v>
-      </c>
-      <c r="Q371" s="4">
-        <v>3.0073218340424859</v>
-      </c>
-    </row>
-    <row r="372" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A372" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="B372" s="4">
-        <v>5.7426641625522477</v>
-      </c>
-      <c r="C372" s="4">
-        <v>2.7676320562397736</v>
-      </c>
-      <c r="D372" s="4">
-        <v>4.4722623444648528</v>
-      </c>
-      <c r="E372" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F372" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G372" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H372" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I372" s="4">
-        <v>1.7549016254479106</v>
-      </c>
-      <c r="J372" s="4">
-        <v>2.4382555521200584</v>
-      </c>
-      <c r="K372" s="4">
-        <v>1.524586403070656</v>
-      </c>
-      <c r="L372" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M372" s="4">
-        <v>0.22156399358652293</v>
-      </c>
-      <c r="N372" s="4">
-        <v>0.10650104950426591</v>
-      </c>
-      <c r="O372" s="4">
-        <v>1.0454711672112358</v>
-      </c>
-      <c r="P372" s="4">
-        <v>2.7320294291017015</v>
-      </c>
-      <c r="Q372" s="4">
-        <v>2.5426740923894036</v>
-      </c>
-    </row>
-    <row r="373" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A373" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B373" s="4">
-        <v>6.2479275134435852</v>
-      </c>
-      <c r="C373" s="4">
-        <v>0.48115291697910012</v>
-      </c>
-      <c r="D373" s="4">
-        <v>1.3692904937527501</v>
-      </c>
-      <c r="E373" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F373" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G373" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H373" s="4">
-        <v>1.9720545336050099</v>
-      </c>
-      <c r="I373" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J373" s="4">
-        <v>3.2333335858711818</v>
-      </c>
-      <c r="K373" s="4">
-        <v>0.24208907364138785</v>
-      </c>
-      <c r="L373" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M373" s="4">
-        <v>0.65861159110681988</v>
-      </c>
-      <c r="N373" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O373" s="4">
-        <v>1.245057583003307</v>
-      </c>
-      <c r="P373" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q373" s="4">
-        <v>3.4007442575478724</v>
-      </c>
-    </row>
-    <row r="374" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A374" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B374" s="4">
-        <v>6.4519719181730801</v>
-      </c>
-      <c r="C374" s="4">
-        <v>2.665684164504766</v>
-      </c>
-      <c r="D374" s="4">
-        <v>0.60699707295601668</v>
-      </c>
-      <c r="E374" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F374" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G374" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H374" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I374" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J374" s="4">
-        <v>0.95830472161217384</v>
-      </c>
-      <c r="K374" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L374" s="4">
-        <v>7.3669852203128411E-2</v>
-      </c>
-      <c r="M374" s="4">
-        <v>1.1384621719923778</v>
-      </c>
-      <c r="N374" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O374" s="4">
-        <v>1.3627273557098056</v>
-      </c>
-      <c r="P374" s="4">
-        <v>1.2368008115725067</v>
-      </c>
-      <c r="Q374" s="4">
-        <v>1.7908292423207046</v>
-      </c>
-    </row>
-    <row r="375" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A375" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="B375" s="4">
-        <v>2.4071283613790579</v>
-      </c>
-      <c r="C375" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D375" s="4">
-        <v>1.1064029378028002</v>
-      </c>
-      <c r="E375" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F375" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G375" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H375" s="4">
-        <v>3.2447539306566346</v>
-      </c>
-      <c r="I375" s="4">
-        <v>0.52343724714559092</v>
-      </c>
-      <c r="J375" s="4">
-        <v>2.2501900917329718</v>
-      </c>
-      <c r="K375" s="4">
-        <v>1.263990149519552</v>
-      </c>
-      <c r="L375" s="4">
-        <v>8.3577132953648894E-2</v>
-      </c>
-      <c r="M375" s="4">
-        <v>6.1371694071634826</v>
-      </c>
-      <c r="N375" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O375" s="4">
-        <v>1.263990149519552</v>
-      </c>
-      <c r="P375" s="4">
-        <v>1.5744073186532239</v>
-      </c>
-      <c r="Q375" s="4">
-        <v>3.111721635221782</v>
-      </c>
-    </row>
-    <row r="376" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A376" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B376" s="4">
-        <v>2.5903975565471251</v>
-      </c>
-      <c r="C376" s="4">
-        <v>0.91195361506137096</v>
-      </c>
-      <c r="D376" s="4">
-        <v>0.33206732611463241</v>
-      </c>
-      <c r="E376" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F376" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G376" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H376" s="4">
-        <v>0.78903623003391155</v>
-      </c>
-      <c r="I376" s="4">
-        <v>0.44780121277899149</v>
-      </c>
-      <c r="J376" s="4">
-        <v>1.6670615948046814</v>
-      </c>
-      <c r="K376" s="4">
-        <v>5.3436538172792991</v>
-      </c>
-      <c r="L376" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M376" s="4">
-        <v>5.4956959901779987</v>
-      </c>
-      <c r="N376" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O376" s="4">
-        <v>1.9068594792362739</v>
-      </c>
-      <c r="P376" s="4">
-        <v>2.334567905530835</v>
-      </c>
-      <c r="Q376" s="4">
-        <v>6.8365366459617341E-2</v>
-      </c>
-    </row>
-    <row r="377" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A377" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="B377" s="4">
-        <v>2.4124986284425072</v>
-      </c>
-      <c r="C377" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D377" s="4">
-        <v>0.57379413643588162</v>
-      </c>
-      <c r="E377" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F377" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G377" s="4">
-        <v>6.9319846619416217E-2</v>
-      </c>
-      <c r="H377" s="4">
-        <v>0.96093814703431712</v>
-      </c>
-      <c r="I377" s="4">
-        <v>9.511887896221638E-2</v>
-      </c>
-      <c r="J377" s="4">
-        <v>1.5212682679655665</v>
-      </c>
-      <c r="K377" s="4">
-        <v>4.1940394695201153</v>
-      </c>
-      <c r="L377" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M377" s="4">
-        <v>6.2171078052321107</v>
-      </c>
-      <c r="N377" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O377" s="4">
-        <v>0.34349581125381207</v>
-      </c>
-      <c r="P377" s="4">
-        <v>1.1151536343657837</v>
-      </c>
-      <c r="Q377" s="4">
-        <v>0.16499428561124574</v>
-      </c>
-    </row>
-    <row r="378" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A378" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="B378" s="4">
-        <v>5.5962400298433419</v>
-      </c>
-      <c r="C378" s="4">
-        <v>2.2052910314613405</v>
-      </c>
-      <c r="D378" s="4">
-        <v>2.4394990818284743</v>
-      </c>
-      <c r="E378" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F378" s="4">
-        <v>0.37360333995838396</v>
-      </c>
-      <c r="G378" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H378" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I378" s="4">
-        <v>0.5014809176495888</v>
-      </c>
-      <c r="J378" s="4">
-        <v>4.0092155592161074</v>
-      </c>
-      <c r="K378" s="4">
-        <v>0.23327873353706935</v>
-      </c>
-      <c r="L378" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M378" s="4">
-        <v>0.43403497397325846</v>
-      </c>
-      <c r="N378" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O378" s="4">
-        <v>1.167998819770778</v>
-      </c>
-      <c r="P378" s="4">
-        <v>2.9215809839509097</v>
-      </c>
-      <c r="Q378" s="4">
-        <v>4.4210923637002928</v>
-      </c>
-    </row>
-    <row r="379" spans="1:17" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A379" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="B379" s="6">
-        <v>6.0213918650521947</v>
-      </c>
-      <c r="C379" s="6">
-        <v>4.8203192546349598</v>
-      </c>
-      <c r="D379" s="6">
-        <v>3.2252206814872664</v>
-      </c>
-      <c r="E379" s="6">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F379" s="6">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G379" s="6">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H379" s="6">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I379" s="6">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J379" s="6">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="K379" s="6">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L379" s="6">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M379" s="6">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N379" s="6">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O379" s="6">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P379" s="6">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q379" s="6">
-        <v>0.52562836133875401</v>
-      </c>
-    </row>
-    <row r="380" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A380" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="B380" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="C380" s="4">
-        <v>6.3696434218432785</v>
-      </c>
-      <c r="D380" s="4">
-        <v>1.268105395381216</v>
-      </c>
-      <c r="E380" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F380" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G380" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H380" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I380" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J380" s="4">
-        <v>0.76911611776991273</v>
-      </c>
-      <c r="K380" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="L380" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M380" s="4">
-        <v>3.9149956452455741</v>
-      </c>
-      <c r="N380" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O380" s="4">
-        <v>1.268105395381216</v>
-      </c>
-      <c r="P380" s="4">
-        <v>0.76911611776991273</v>
-      </c>
-      <c r="Q380" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="381" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A381" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="B381" s="4">
-        <v>6.2357074247890845</v>
-      </c>
-      <c r="C381" s="4">
-        <v>2.2768402053588246</v>
-      </c>
-      <c r="D381" s="4">
-        <v>3.9766926265079312</v>
-      </c>
-      <c r="E381" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F381" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G381" s="4">
-        <v>1.5474877953024935</v>
-      </c>
-      <c r="H381" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I381" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J381" s="4">
-        <v>1.5474877953024935</v>
-      </c>
-      <c r="K381" s="4">
-        <v>1.1903312121041496</v>
-      </c>
-      <c r="L381" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M381" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N381" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O381" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P381" s="4">
-        <v>1.5474877953024935</v>
-      </c>
-      <c r="Q381" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="382" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A382" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="B382" s="4">
-        <v>3.8541491335365454</v>
-      </c>
-      <c r="C382" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="D382" s="4">
-        <v>1.5474877953024933</v>
-      </c>
-      <c r="E382" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F382" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G382" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H382" s="4">
-        <v>2.2768402053588241</v>
-      </c>
-      <c r="I382" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J382" s="4">
-        <v>3.8541491335365454</v>
-      </c>
-      <c r="K382" s="4">
-        <v>5.3710226444155325</v>
-      </c>
-      <c r="L382" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M382" s="4">
-        <v>3.648288436089985</v>
-      </c>
-      <c r="N382" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O382" s="4">
-        <v>4.0342699020847457</v>
-      </c>
-      <c r="P382" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q382" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="383" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A383" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="B383" s="4">
-        <v>6.1215843030494757</v>
-      </c>
-      <c r="C383" s="4">
-        <v>3.8147447614745822</v>
-      </c>
-      <c r="D383" s="4">
-        <v>1.5659793973535834</v>
-      </c>
-      <c r="E383" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F383" s="4">
-        <v>0.72560573200165868</v>
-      </c>
-      <c r="G383" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="H383" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="I383" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J383" s="4">
-        <v>2.2991182119792763</v>
-      </c>
-      <c r="K383" s="4">
-        <v>3.67408839119414</v>
-      </c>
-      <c r="L383" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M383" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N383" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O383" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="P383" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q383" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
-    <row r="384" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A384" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="B384" s="4">
-        <v>5.81817789135214</v>
-      </c>
-      <c r="C384" s="4">
-        <v>1.7696188114849576</v>
-      </c>
-      <c r="D384" s="4">
-        <v>3.5660081749936556</v>
-      </c>
-      <c r="E384" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="F384" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="G384" s="4">
-        <v>1.7696188114849576</v>
-      </c>
-      <c r="H384" s="4">
-        <v>3.237829065944116</v>
-      </c>
-      <c r="I384" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="J384" s="4">
-        <v>2.2061611505780321</v>
-      </c>
-      <c r="K384" s="4">
-        <v>3.411230196301541</v>
-      </c>
-      <c r="L384" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="M384" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="N384" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="O384" s="4">
-        <v>3.0407023369431654</v>
-      </c>
-      <c r="P384" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-      <c r="Q384" s="4">
-        <v>3.2034265038149171E-16</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>